<commit_message>
Distributed officer training law levels
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51056204-7DAE-446F-877E-241E1CA9E7FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AF22D0-B587-4892-AF09-BC9622FA10DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
   <si>
     <t>TAG</t>
   </si>
@@ -829,6 +829,9 @@
   </si>
   <si>
     <t xml:space="preserve">SIA = "countries/Siam.txt" </t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -870,13 +873,89 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="20">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -929,6 +1008,66 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -951,12 +1090,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{10BD23E6-60AB-42C7-B043-A8B30FF8C033}" name="Taulukko2" displayName="Taulukko2" ref="B2:P253" totalsRowShown="0">
-  <autoFilter ref="B2:P253" xr:uid="{6DDEF623-4240-4F7B-A4DC-C137388F3BBA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{10BD23E6-60AB-42C7-B043-A8B30FF8C033}" name="Taulukko2" displayName="Taulukko2" ref="B2:Q253" totalsRowShown="0">
+  <autoFilter ref="B2:Q253" xr:uid="{6DDEF623-4240-4F7B-A4DC-C137388F3BBA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P253">
     <sortCondition ref="B2:B253"/>
   </sortState>
-  <tableColumns count="15">
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{0F370F1D-33D6-4690-B3B1-6018D18D0D34}" name="TAG"/>
     <tableColumn id="2" xr3:uid="{A251529F-C198-4882-980D-186989E9B99C}" name="Units 1"/>
     <tableColumn id="3" xr3:uid="{7E1D6517-8E7B-4427-B6C9-14389192DE8B}" name="Is Major 1"/>
@@ -984,6 +1123,7 @@
     <tableColumn id="15" xr3:uid="{AD6381E7-3290-44E4-9E98-E7E9063F54F9}" name="DeltaFM">
       <calculatedColumnFormula>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1252,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P253"/>
+  <dimension ref="B2:Q253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1417,7 @@
     <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1323,8 +1463,11 @@
       <c r="P2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>213</v>
       </c>
@@ -1358,8 +1501,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>214</v>
       </c>
@@ -1393,8 +1537,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>50</v>
       </c>
@@ -1428,8 +1573,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>215</v>
       </c>
@@ -1463,8 +1609,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>216</v>
       </c>
@@ -1498,8 +1645,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>155</v>
       </c>
@@ -1533,8 +1681,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>51</v>
       </c>
@@ -1568,8 +1717,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1606,8 +1756,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>156</v>
       </c>
@@ -1641,8 +1792,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>217</v>
       </c>
@@ -1676,8 +1828,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>52</v>
       </c>
@@ -1711,8 +1864,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>136</v>
       </c>
@@ -1746,8 +1900,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>53</v>
       </c>
@@ -1787,8 +1942,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>112</v>
       </c>
@@ -1822,8 +1978,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -1857,8 +2014,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>54</v>
       </c>
@@ -1892,8 +2050,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>123</v>
       </c>
@@ -1927,8 +2086,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>218</v>
       </c>
@@ -1962,8 +2122,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>85</v>
       </c>
@@ -1997,8 +2158,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>124</v>
       </c>
@@ -2032,8 +2194,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -2073,8 +2236,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>157</v>
       </c>
@@ -2108,8 +2272,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>158</v>
       </c>
@@ -2143,8 +2308,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>55</v>
       </c>
@@ -2184,8 +2350,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>86</v>
       </c>
@@ -2219,8 +2386,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>56</v>
       </c>
@@ -2254,8 +2422,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>4</v>
       </c>
@@ -2295,8 +2464,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q29" s="1"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>125</v>
       </c>
@@ -2330,8 +2500,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q30" s="1"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>137</v>
       </c>
@@ -2365,8 +2536,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q31" s="1"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>5</v>
       </c>
@@ -2400,8 +2572,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q32" s="1"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>159</v>
       </c>
@@ -2435,8 +2608,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q33" s="1"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>138</v>
       </c>
@@ -2470,8 +2644,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q34" s="1"/>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>87</v>
       </c>
@@ -2505,8 +2680,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q35" s="1"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>88</v>
       </c>
@@ -2540,8 +2716,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q36" s="1"/>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>6</v>
       </c>
@@ -2578,8 +2755,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q37" s="1"/>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>160</v>
       </c>
@@ -2613,8 +2791,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q38" s="1"/>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>161</v>
       </c>
@@ -2648,8 +2827,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q39" s="1"/>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>119</v>
       </c>
@@ -2689,8 +2869,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>162</v>
       </c>
@@ -2724,8 +2905,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q41" s="1"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>7</v>
       </c>
@@ -2759,8 +2941,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q42" s="1"/>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>89</v>
       </c>
@@ -2794,8 +2977,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q43" s="1"/>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>163</v>
       </c>
@@ -2829,8 +3013,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q44" s="1"/>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>164</v>
       </c>
@@ -2864,8 +3049,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q45" s="1"/>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>49</v>
       </c>
@@ -2899,8 +3085,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q46" s="1"/>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>90</v>
       </c>
@@ -2946,8 +3133,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q47" s="1"/>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>139</v>
       </c>
@@ -2981,8 +3169,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q48" s="1"/>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>165</v>
       </c>
@@ -3016,8 +3205,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q49" s="1"/>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>166</v>
       </c>
@@ -3051,8 +3241,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q50" s="1"/>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>140</v>
       </c>
@@ -3086,8 +3277,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q51" s="1"/>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>167</v>
       </c>
@@ -3121,8 +3313,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q52" s="1"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>141</v>
       </c>
@@ -3156,8 +3349,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q53" s="1"/>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>8</v>
       </c>
@@ -3191,8 +3385,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q54" s="1"/>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>9</v>
       </c>
@@ -3229,8 +3424,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q55" s="1"/>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>122</v>
       </c>
@@ -3264,8 +3460,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q56" s="1"/>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>126</v>
       </c>
@@ -3299,8 +3496,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q57" s="1"/>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>10</v>
       </c>
@@ -3334,8 +3532,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q58" s="1"/>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>11</v>
       </c>
@@ -3375,8 +3574,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q59" s="1"/>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>219</v>
       </c>
@@ -3410,8 +3610,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q60" s="1"/>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>12</v>
       </c>
@@ -3451,8 +3652,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q61" s="1"/>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>168</v>
       </c>
@@ -3486,8 +3688,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q62" s="1"/>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>127</v>
       </c>
@@ -3521,8 +3724,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q63" s="1"/>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>128</v>
       </c>
@@ -3556,8 +3760,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q64" s="1"/>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>169</v>
       </c>
@@ -3591,8 +3796,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q65" s="1"/>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>57</v>
       </c>
@@ -3626,8 +3832,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q66" s="1"/>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>142</v>
       </c>
@@ -3661,8 +3868,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q67" s="1"/>
+    </row>
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>170</v>
       </c>
@@ -3696,8 +3904,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q68" s="1"/>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>171</v>
       </c>
@@ -3731,8 +3940,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q69" s="1"/>
+    </row>
+    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>143</v>
       </c>
@@ -3766,8 +3976,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q70" s="1"/>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>13</v>
       </c>
@@ -3810,8 +4021,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q71" s="1"/>
+    </row>
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>172</v>
       </c>
@@ -3845,8 +4057,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q72" s="1"/>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>14</v>
       </c>
@@ -3883,8 +4096,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q73" s="1"/>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>173</v>
       </c>
@@ -3918,8 +4132,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q74" s="1"/>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>113</v>
       </c>
@@ -3953,8 +4168,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q75" s="1"/>
+    </row>
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>15</v>
       </c>
@@ -3988,8 +4204,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q76" s="1"/>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>16</v>
       </c>
@@ -4029,8 +4246,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q77" s="1"/>
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>220</v>
       </c>
@@ -4064,8 +4282,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q78" s="1"/>
+    </row>
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>17</v>
       </c>
@@ -4099,8 +4318,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q79" s="1"/>
+    </row>
+    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>174</v>
       </c>
@@ -4134,8 +4354,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q80" s="1"/>
+    </row>
+    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>175</v>
       </c>
@@ -4169,8 +4390,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q81" s="1"/>
+    </row>
+    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>176</v>
       </c>
@@ -4204,8 +4426,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q82" s="1"/>
+    </row>
+    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>58</v>
       </c>
@@ -4239,8 +4462,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q83" s="1"/>
+    </row>
+    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>18</v>
       </c>
@@ -4286,8 +4510,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q84" s="1"/>
+    </row>
+    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>221</v>
       </c>
@@ -4321,8 +4546,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q85" s="1"/>
+    </row>
+    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>222</v>
       </c>
@@ -4356,8 +4582,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q86" s="1"/>
+    </row>
+    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>129</v>
       </c>
@@ -4391,8 +4618,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q87" s="1"/>
+    </row>
+    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>19</v>
       </c>
@@ -4432,8 +4660,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q88" s="1"/>
+    </row>
+    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>144</v>
       </c>
@@ -4467,8 +4696,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q89" s="1"/>
+    </row>
+    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>177</v>
       </c>
@@ -4502,8 +4732,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q90" s="1"/>
+    </row>
+    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>178</v>
       </c>
@@ -4537,8 +4768,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q91" s="1"/>
+    </row>
+    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>145</v>
       </c>
@@ -4572,8 +4804,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q92" s="1"/>
+    </row>
+    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>130</v>
       </c>
@@ -4607,8 +4840,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q93" s="1"/>
+    </row>
+    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>223</v>
       </c>
@@ -4642,8 +4876,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q94" s="1"/>
+    </row>
+    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>59</v>
       </c>
@@ -4677,8 +4912,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q95" s="1"/>
+    </row>
+    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>224</v>
       </c>
@@ -4715,8 +4951,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q96" s="1"/>
+    </row>
+    <row r="97" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>91</v>
       </c>
@@ -4756,8 +4993,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q97" s="1"/>
+    </row>
+    <row r="98" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>25</v>
       </c>
@@ -4791,8 +5029,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q98" s="1"/>
+    </row>
+    <row r="99" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>20</v>
       </c>
@@ -4832,8 +5071,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q99" s="1"/>
+    </row>
+    <row r="100" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>146</v>
       </c>
@@ -4867,8 +5107,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q100" s="1"/>
+    </row>
+    <row r="101" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>225</v>
       </c>
@@ -4902,8 +5143,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q101" s="1"/>
+    </row>
+    <row r="102" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>226</v>
       </c>
@@ -4937,8 +5179,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q102" s="1"/>
+    </row>
+    <row r="103" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>21</v>
       </c>
@@ -4978,8 +5221,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q103" s="1"/>
+    </row>
+    <row r="104" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>22</v>
       </c>
@@ -5019,8 +5263,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q104" s="1"/>
+    </row>
+    <row r="105" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>92</v>
       </c>
@@ -5054,8 +5299,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q105" s="1"/>
+    </row>
+    <row r="106" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>23</v>
       </c>
@@ -5089,8 +5335,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q106" s="1"/>
+    </row>
+    <row r="107" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>60</v>
       </c>
@@ -5124,8 +5371,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q107" s="1"/>
+    </row>
+    <row r="108" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>227</v>
       </c>
@@ -5159,8 +5407,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q108" s="1"/>
+    </row>
+    <row r="109" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>61</v>
       </c>
@@ -5194,8 +5443,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q109" s="1"/>
+    </row>
+    <row r="110" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>24</v>
       </c>
@@ -5235,8 +5485,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q110" s="1"/>
+    </row>
+    <row r="111" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>131</v>
       </c>
@@ -5270,8 +5521,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q111" s="1"/>
+    </row>
+    <row r="112" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>62</v>
       </c>
@@ -5311,8 +5563,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q112" s="1"/>
+    </row>
+    <row r="113" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>63</v>
       </c>
@@ -5346,8 +5599,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q113" s="1"/>
+    </row>
+    <row r="114" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>228</v>
       </c>
@@ -5381,8 +5635,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q114" s="1"/>
+    </row>
+    <row r="115" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>93</v>
       </c>
@@ -5416,8 +5671,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q115" s="1"/>
+    </row>
+    <row r="116" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>94</v>
       </c>
@@ -5451,8 +5707,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q116" s="1"/>
+    </row>
+    <row r="117" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>64</v>
       </c>
@@ -5492,8 +5749,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q117" s="1"/>
+    </row>
+    <row r="118" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>179</v>
       </c>
@@ -5527,8 +5785,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q118" s="1"/>
+    </row>
+    <row r="119" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>95</v>
       </c>
@@ -5562,8 +5821,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q119" s="1"/>
+    </row>
+    <row r="120" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>26</v>
       </c>
@@ -5597,8 +5857,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q120" s="1"/>
+    </row>
+    <row r="121" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>229</v>
       </c>
@@ -5632,8 +5893,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q121" s="1"/>
+    </row>
+    <row r="122" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>65</v>
       </c>
@@ -5667,8 +5929,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q122" s="1"/>
+    </row>
+    <row r="123" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>66</v>
       </c>
@@ -5708,8 +5971,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q123" s="1"/>
+    </row>
+    <row r="124" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>96</v>
       </c>
@@ -5743,8 +6007,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q124" s="1"/>
+    </row>
+    <row r="125" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>27</v>
       </c>
@@ -5781,8 +6046,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q125" s="1"/>
+    </row>
+    <row r="126" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>180</v>
       </c>
@@ -5816,8 +6082,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q126" s="1"/>
+    </row>
+    <row r="127" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>67</v>
       </c>
@@ -5851,8 +6118,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q127" s="1"/>
+    </row>
+    <row r="128" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>181</v>
       </c>
@@ -5886,8 +6154,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q128" s="1"/>
+    </row>
+    <row r="129" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>182</v>
       </c>
@@ -5921,8 +6190,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q129" s="1"/>
+    </row>
+    <row r="130" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>28</v>
       </c>
@@ -5959,8 +6229,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q130" s="1"/>
+    </row>
+    <row r="131" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>231</v>
       </c>
@@ -5994,8 +6265,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q131" s="1"/>
+    </row>
+    <row r="132" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>68</v>
       </c>
@@ -6029,8 +6301,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q132" s="1"/>
+    </row>
+    <row r="133" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>230</v>
       </c>
@@ -6064,8 +6337,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q133" s="1"/>
+    </row>
+    <row r="134" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>29</v>
       </c>
@@ -6105,8 +6379,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q134" s="1"/>
+    </row>
+    <row r="135" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>183</v>
       </c>
@@ -6140,8 +6415,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q135" s="1"/>
+    </row>
+    <row r="136" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>184</v>
       </c>
@@ -6175,8 +6451,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q136" s="1"/>
+    </row>
+    <row r="137" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>185</v>
       </c>
@@ -6210,8 +6487,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q137" s="1"/>
+    </row>
+    <row r="138" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>97</v>
       </c>
@@ -6245,8 +6523,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q138" s="1"/>
+    </row>
+    <row r="139" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>120</v>
       </c>
@@ -6280,8 +6559,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q139" s="1"/>
+    </row>
+    <row r="140" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>114</v>
       </c>
@@ -6315,8 +6595,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q140" s="1"/>
+    </row>
+    <row r="141" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>232</v>
       </c>
@@ -6350,8 +6631,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q141" s="1"/>
+    </row>
+    <row r="142" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>98</v>
       </c>
@@ -6385,8 +6667,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q142" s="1"/>
+    </row>
+    <row r="143" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>30</v>
       </c>
@@ -6420,8 +6703,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q143" s="1"/>
+    </row>
+    <row r="144" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>186</v>
       </c>
@@ -6455,8 +6739,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q144" s="1"/>
+    </row>
+    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>31</v>
       </c>
@@ -6490,8 +6775,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q145" s="1"/>
+    </row>
+    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>32</v>
       </c>
@@ -6525,8 +6811,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q146" s="1"/>
+    </row>
+    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>99</v>
       </c>
@@ -6560,8 +6847,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q147" s="1"/>
+    </row>
+    <row r="148" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>187</v>
       </c>
@@ -6595,8 +6883,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q148" s="1"/>
+    </row>
+    <row r="149" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>188</v>
       </c>
@@ -6630,8 +6919,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q149" s="1"/>
+    </row>
+    <row r="150" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>189</v>
       </c>
@@ -6665,8 +6955,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q150" s="1"/>
+    </row>
+    <row r="151" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>190</v>
       </c>
@@ -6700,8 +6991,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q151" s="1"/>
+    </row>
+    <row r="152" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>33</v>
       </c>
@@ -6735,8 +7027,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q152" s="1"/>
+    </row>
+    <row r="153" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>69</v>
       </c>
@@ -6770,8 +7063,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q153" s="1"/>
+    </row>
+    <row r="154" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>100</v>
       </c>
@@ -6805,8 +7099,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q154" s="1"/>
+    </row>
+    <row r="155" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>191</v>
       </c>
@@ -6840,8 +7135,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q155" s="1"/>
+    </row>
+    <row r="156" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>147</v>
       </c>
@@ -6875,8 +7171,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q156" s="1"/>
+    </row>
+    <row r="157" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>192</v>
       </c>
@@ -6910,8 +7207,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q157" s="1"/>
+    </row>
+    <row r="158" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>101</v>
       </c>
@@ -6945,8 +7243,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q158" s="1"/>
+    </row>
+    <row r="159" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>70</v>
       </c>
@@ -6986,8 +7285,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q159" s="1"/>
+    </row>
+    <row r="160" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>34</v>
       </c>
@@ -7027,8 +7327,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q160" s="1"/>
+    </row>
+    <row r="161" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>233</v>
       </c>
@@ -7062,8 +7363,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q161" s="1"/>
+    </row>
+    <row r="162" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>234</v>
       </c>
@@ -7097,8 +7399,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q162" s="1"/>
+    </row>
+    <row r="163" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>115</v>
       </c>
@@ -7132,8 +7435,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q163" s="1"/>
+    </row>
+    <row r="164" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>71</v>
       </c>
@@ -7167,8 +7471,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q164" s="1"/>
+    </row>
+    <row r="165" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>72</v>
       </c>
@@ -7202,8 +7507,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q165" s="1"/>
+    </row>
+    <row r="166" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>73</v>
       </c>
@@ -7237,8 +7543,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q166" s="1"/>
+    </row>
+    <row r="167" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>148</v>
       </c>
@@ -7272,8 +7579,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q167" s="1"/>
+    </row>
+    <row r="168" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>116</v>
       </c>
@@ -7307,8 +7615,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q168" s="1"/>
+    </row>
+    <row r="169" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>149</v>
       </c>
@@ -7342,8 +7651,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q169" s="1"/>
+    </row>
+    <row r="170" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>150</v>
       </c>
@@ -7377,8 +7687,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q170" s="1"/>
+    </row>
+    <row r="171" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>74</v>
       </c>
@@ -7418,8 +7729,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="172" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q171" s="1"/>
+    </row>
+    <row r="172" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>102</v>
       </c>
@@ -7453,8 +7765,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q172" s="1"/>
+    </row>
+    <row r="173" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>235</v>
       </c>
@@ -7488,8 +7801,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q173" s="1"/>
+    </row>
+    <row r="174" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>117</v>
       </c>
@@ -7523,8 +7837,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q174" s="1"/>
+    </row>
+    <row r="175" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>236</v>
       </c>
@@ -7558,8 +7873,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q175" s="1"/>
+    </row>
+    <row r="176" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>35</v>
       </c>
@@ -7599,8 +7915,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q176" s="1"/>
+    </row>
+    <row r="177" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>36</v>
       </c>
@@ -7640,8 +7957,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q177" s="1"/>
+    </row>
+    <row r="178" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>151</v>
       </c>
@@ -7675,8 +7993,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q178" s="1"/>
+    </row>
+    <row r="179" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>237</v>
       </c>
@@ -7710,8 +8029,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q179" s="1"/>
+    </row>
+    <row r="180" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>75</v>
       </c>
@@ -7745,8 +8065,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q180" s="1"/>
+    </row>
+    <row r="181" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>76</v>
       </c>
@@ -7780,8 +8101,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q181" s="1"/>
+    </row>
+    <row r="182" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>250</v>
       </c>
@@ -7815,8 +8137,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q182" s="1"/>
+    </row>
+    <row r="183" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>103</v>
       </c>
@@ -7853,8 +8176,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q183" s="1"/>
+    </row>
+    <row r="184" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>238</v>
       </c>
@@ -7888,8 +8212,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q184" s="1"/>
+    </row>
+    <row r="185" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>239</v>
       </c>
@@ -7923,8 +8248,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q185" s="1"/>
+    </row>
+    <row r="186" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>37</v>
       </c>
@@ -7961,8 +8287,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q186" s="1"/>
+    </row>
+    <row r="187" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>193</v>
       </c>
@@ -7996,8 +8323,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q187" s="1"/>
+    </row>
+    <row r="188" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>194</v>
       </c>
@@ -8031,8 +8359,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q188" s="1"/>
+    </row>
+    <row r="189" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>195</v>
       </c>
@@ -8066,8 +8395,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q189" s="1"/>
+    </row>
+    <row r="190" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>77</v>
       </c>
@@ -8113,8 +8443,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q190" s="1"/>
+    </row>
+    <row r="191" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>38</v>
       </c>
@@ -8148,8 +8479,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q191" s="1"/>
+    </row>
+    <row r="192" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>39</v>
       </c>
@@ -8183,8 +8515,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q192" s="1"/>
+    </row>
+    <row r="193" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>241</v>
       </c>
@@ -8218,8 +8551,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q193" s="1"/>
+    </row>
+    <row r="194" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>196</v>
       </c>
@@ -8253,8 +8587,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q194" s="1"/>
+    </row>
+    <row r="195" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>40</v>
       </c>
@@ -8288,8 +8623,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="196" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q195" s="1"/>
+    </row>
+    <row r="196" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>197</v>
       </c>
@@ -8323,8 +8659,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q196" s="1"/>
+    </row>
+    <row r="197" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>198</v>
       </c>
@@ -8358,8 +8695,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q197" s="1"/>
+    </row>
+    <row r="198" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>240</v>
       </c>
@@ -8393,8 +8731,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="199" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q198" s="1"/>
+    </row>
+    <row r="199" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>104</v>
       </c>
@@ -8428,8 +8767,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q199" s="1"/>
+    </row>
+    <row r="200" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>265</v>
       </c>
@@ -8463,8 +8803,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q200" s="1"/>
+    </row>
+    <row r="201" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>199</v>
       </c>
@@ -8498,8 +8839,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q201" s="1"/>
+    </row>
+    <row r="202" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>105</v>
       </c>
@@ -8533,8 +8875,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q202" s="1"/>
+    </row>
+    <row r="203" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
         <v>41</v>
       </c>
@@ -8571,8 +8914,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q203" s="1"/>
+    </row>
+    <row r="204" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
         <v>42</v>
       </c>
@@ -8609,8 +8953,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q204" s="1"/>
+    </row>
+    <row r="205" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>200</v>
       </c>
@@ -8644,8 +8989,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q205" s="1"/>
+    </row>
+    <row r="206" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>242</v>
       </c>
@@ -8679,8 +9025,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q206" s="1"/>
+    </row>
+    <row r="207" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>118</v>
       </c>
@@ -8714,8 +9061,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q207" s="1"/>
+    </row>
+    <row r="208" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>201</v>
       </c>
@@ -8749,8 +9097,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="209" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q208" s="1"/>
+    </row>
+    <row r="209" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>243</v>
       </c>
@@ -8784,8 +9133,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q209" s="1"/>
+    </row>
+    <row r="210" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>43</v>
       </c>
@@ -8831,8 +9181,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q210" s="1"/>
+    </row>
+    <row r="211" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>44</v>
       </c>
@@ -8872,8 +9223,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q211" s="1"/>
+    </row>
+    <row r="212" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>244</v>
       </c>
@@ -8907,8 +9259,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q212" s="1"/>
+    </row>
+    <row r="213" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
         <v>106</v>
       </c>
@@ -8942,8 +9295,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q213" s="1"/>
+    </row>
+    <row r="214" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
         <v>202</v>
       </c>
@@ -8977,8 +9331,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q214" s="1"/>
+    </row>
+    <row r="215" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
         <v>203</v>
       </c>
@@ -9012,8 +9367,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q215" s="1"/>
+    </row>
+    <row r="216" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
         <v>132</v>
       </c>
@@ -9047,8 +9403,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q216" s="1"/>
+    </row>
+    <row r="217" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>133</v>
       </c>
@@ -9082,8 +9439,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q217" s="1"/>
+    </row>
+    <row r="218" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
         <v>134</v>
       </c>
@@ -9117,8 +9475,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q218" s="1"/>
+    </row>
+    <row r="219" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
         <v>204</v>
       </c>
@@ -9152,8 +9511,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q219" s="1"/>
+    </row>
+    <row r="220" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
         <v>152</v>
       </c>
@@ -9187,8 +9547,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q220" s="1"/>
+    </row>
+    <row r="221" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
         <v>205</v>
       </c>
@@ -9222,8 +9583,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q221" s="1"/>
+    </row>
+    <row r="222" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
         <v>45</v>
       </c>
@@ -9257,8 +9619,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q222" s="1"/>
+    </row>
+    <row r="223" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
         <v>46</v>
       </c>
@@ -9292,8 +9655,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q223" s="1"/>
+    </row>
+    <row r="224" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
         <v>245</v>
       </c>
@@ -9327,8 +9691,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q224" s="1"/>
+    </row>
+    <row r="225" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
         <v>78</v>
       </c>
@@ -9362,8 +9727,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q225" s="1"/>
+    </row>
+    <row r="226" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
         <v>79</v>
       </c>
@@ -9397,8 +9763,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q226" s="1"/>
+    </row>
+    <row r="227" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
         <v>107</v>
       </c>
@@ -9432,8 +9799,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q227" s="1"/>
+    </row>
+    <row r="228" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
         <v>80</v>
       </c>
@@ -9473,8 +9841,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q228" s="1"/>
+    </row>
+    <row r="229" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
         <v>246</v>
       </c>
@@ -9508,8 +9877,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q229" s="1"/>
+    </row>
+    <row r="230" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
         <v>108</v>
       </c>
@@ -9543,8 +9913,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="231" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q230" s="1"/>
+    </row>
+    <row r="231" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
         <v>109</v>
       </c>
@@ -9578,8 +9949,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q231" s="1"/>
+    </row>
+    <row r="232" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
         <v>206</v>
       </c>
@@ -9613,8 +9985,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q232" s="1"/>
+    </row>
+    <row r="233" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
         <v>207</v>
       </c>
@@ -9648,8 +10021,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q233" s="1"/>
+    </row>
+    <row r="234" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
         <v>135</v>
       </c>
@@ -9683,8 +10057,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q234" s="1"/>
+    </row>
+    <row r="235" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
         <v>81</v>
       </c>
@@ -9718,8 +10093,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q235" s="1"/>
+    </row>
+    <row r="236" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
         <v>247</v>
       </c>
@@ -9753,8 +10129,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="237" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q236" s="1"/>
+    </row>
+    <row r="237" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
         <v>248</v>
       </c>
@@ -9788,8 +10165,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q237" s="1"/>
+    </row>
+    <row r="238" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
         <v>208</v>
       </c>
@@ -9823,8 +10201,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q238" s="1"/>
+    </row>
+    <row r="239" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
         <v>47</v>
       </c>
@@ -9864,8 +10243,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q239" s="1"/>
+    </row>
+    <row r="240" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
         <v>82</v>
       </c>
@@ -9905,8 +10285,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q240" s="1"/>
+    </row>
+    <row r="241" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
         <v>209</v>
       </c>
@@ -9940,8 +10321,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="242" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q241" s="1"/>
+    </row>
+    <row r="242" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
         <v>48</v>
       </c>
@@ -9975,8 +10357,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="243" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q242" s="1"/>
+    </row>
+    <row r="243" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
         <v>249</v>
       </c>
@@ -10010,8 +10393,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="244" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q243" s="1"/>
+    </row>
+    <row r="244" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
         <v>153</v>
       </c>
@@ -10045,8 +10429,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="245" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q244" s="1"/>
+    </row>
+    <row r="245" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
         <v>121</v>
       </c>
@@ -10092,8 +10477,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="246" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q245" s="1"/>
+    </row>
+    <row r="246" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
         <v>83</v>
       </c>
@@ -10127,8 +10513,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q246" s="1"/>
+    </row>
+    <row r="247" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
         <v>111</v>
       </c>
@@ -10162,8 +10549,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="248" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q247" s="1"/>
+    </row>
+    <row r="248" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
         <v>154</v>
       </c>
@@ -10197,8 +10585,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="249" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q248" s="1"/>
+    </row>
+    <row r="249" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
         <v>210</v>
       </c>
@@ -10232,8 +10621,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q249" s="1"/>
+    </row>
+    <row r="250" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
         <v>110</v>
       </c>
@@ -10267,8 +10657,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q250" s="1"/>
+    </row>
+    <row r="251" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
         <v>84</v>
       </c>
@@ -10302,8 +10693,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q251" s="1"/>
+    </row>
+    <row r="252" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
         <v>211</v>
       </c>
@@ -10337,8 +10729,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q252" s="1"/>
+    </row>
+    <row r="253" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
         <v>212</v>
       </c>
@@ -10372,23 +10765,30 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
+      <c r="Q253" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O3:P253">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q253">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
General Rework - ABK to AQY
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AF22D0-B587-4892-AF09-BC9622FA10DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47366AB1-3542-465C-AFB2-FDAAE93D720A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="270">
   <si>
     <t>TAG</t>
   </si>
@@ -832,6 +832,15 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>ID min</t>
+  </si>
+  <si>
+    <t>ID max</t>
   </si>
 </sst>
 </file>
@@ -882,7 +891,7 @@
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="5">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -893,156 +902,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1090,12 +949,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{10BD23E6-60AB-42C7-B043-A8B30FF8C033}" name="Taulukko2" displayName="Taulukko2" ref="B2:Q253" totalsRowShown="0">
-  <autoFilter ref="B2:Q253" xr:uid="{6DDEF623-4240-4F7B-A4DC-C137388F3BBA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{10BD23E6-60AB-42C7-B043-A8B30FF8C033}" name="Taulukko2" displayName="Taulukko2" ref="B2:S253" totalsRowShown="0">
+  <autoFilter ref="B2:S253" xr:uid="{6DDEF623-4240-4F7B-A4DC-C137388F3BBA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P253">
     <sortCondition ref="B2:B253"/>
   </sortState>
-  <tableColumns count="16">
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{0F370F1D-33D6-4690-B3B1-6018D18D0D34}" name="TAG"/>
     <tableColumn id="2" xr3:uid="{A251529F-C198-4882-980D-186989E9B99C}" name="Units 1"/>
     <tableColumn id="3" xr3:uid="{7E1D6517-8E7B-4427-B6C9-14389192DE8B}" name="Is Major 1"/>
@@ -1124,6 +983,8 @@
       <calculatedColumnFormula>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{C49D052D-3754-49A2-9551-F2176AA27932}" name="ID min"/>
+    <tableColumn id="18" xr3:uid="{8A6F4AEA-EC4E-4C6E-A653-1A392AFA8658}" name="ID max"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1392,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q253"/>
+  <dimension ref="B2:S253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1278,7 @@
     <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1466,8 +1327,14 @@
       <c r="Q2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>268</v>
+      </c>
+      <c r="S2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>213</v>
       </c>
@@ -1501,9 +1368,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>214</v>
       </c>
@@ -1537,9 +1412,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q4" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R4">
+        <v>21</v>
+      </c>
+      <c r="S4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>50</v>
       </c>
@@ -1573,9 +1456,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q5" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R5">
+        <v>41</v>
+      </c>
+      <c r="S5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>215</v>
       </c>
@@ -1609,9 +1500,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R6">
+        <v>61</v>
+      </c>
+      <c r="S6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>216</v>
       </c>
@@ -1645,9 +1544,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q7" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R7">
+        <v>81</v>
+      </c>
+      <c r="S7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>155</v>
       </c>
@@ -1681,9 +1588,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q8" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R8">
+        <v>101</v>
+      </c>
+      <c r="S8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>51</v>
       </c>
@@ -1717,9 +1632,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q9" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R9">
+        <v>121</v>
+      </c>
+      <c r="S9">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1756,9 +1679,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q10" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R10">
+        <v>141</v>
+      </c>
+      <c r="S10">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>156</v>
       </c>
@@ -1792,9 +1723,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q11" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R11">
+        <v>161</v>
+      </c>
+      <c r="S11">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>217</v>
       </c>
@@ -1828,9 +1767,17 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R12">
+        <v>181</v>
+      </c>
+      <c r="S12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>52</v>
       </c>
@@ -1865,8 +1812,14 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>201</v>
+      </c>
+      <c r="S13">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>136</v>
       </c>
@@ -1901,8 +1854,14 @@
         <v>1</v>
       </c>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>221</v>
+      </c>
+      <c r="S14">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>53</v>
       </c>
@@ -1943,8 +1902,14 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>241</v>
+      </c>
+      <c r="S15">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>112</v>
       </c>
@@ -1979,8 +1944,14 @@
         <v>0</v>
       </c>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>261</v>
+      </c>
+      <c r="S16">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -2015,8 +1986,14 @@
         <v>1</v>
       </c>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>281</v>
+      </c>
+      <c r="S17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>54</v>
       </c>
@@ -2051,8 +2028,14 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>301</v>
+      </c>
+      <c r="S18">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>123</v>
       </c>
@@ -2087,8 +2070,14 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>321</v>
+      </c>
+      <c r="S19">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>218</v>
       </c>
@@ -2123,8 +2112,14 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>341</v>
+      </c>
+      <c r="S20">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>85</v>
       </c>
@@ -2159,8 +2154,14 @@
         <v>0</v>
       </c>
       <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>361</v>
+      </c>
+      <c r="S21">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>124</v>
       </c>
@@ -2195,8 +2196,14 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>381</v>
+      </c>
+      <c r="S22">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -2237,8 +2244,14 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>401</v>
+      </c>
+      <c r="S23">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>157</v>
       </c>
@@ -2273,8 +2286,14 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>421</v>
+      </c>
+      <c r="S24">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>158</v>
       </c>
@@ -2309,8 +2328,14 @@
         <v>0</v>
       </c>
       <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <v>441</v>
+      </c>
+      <c r="S25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>55</v>
       </c>
@@ -2351,8 +2376,14 @@
         <v>0</v>
       </c>
       <c r="Q26" s="1"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <v>461</v>
+      </c>
+      <c r="S26">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>86</v>
       </c>
@@ -2387,8 +2418,14 @@
         <v>0</v>
       </c>
       <c r="Q27" s="1"/>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>481</v>
+      </c>
+      <c r="S27">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>56</v>
       </c>
@@ -2423,8 +2460,14 @@
         <v>0</v>
       </c>
       <c r="Q28" s="1"/>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>501</v>
+      </c>
+      <c r="S28">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>4</v>
       </c>
@@ -2465,8 +2508,14 @@
         <v>0</v>
       </c>
       <c r="Q29" s="1"/>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <v>521</v>
+      </c>
+      <c r="S29">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>125</v>
       </c>
@@ -2501,8 +2550,14 @@
         <v>0</v>
       </c>
       <c r="Q30" s="1"/>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <v>541</v>
+      </c>
+      <c r="S30">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>137</v>
       </c>
@@ -2537,8 +2592,14 @@
         <v>0</v>
       </c>
       <c r="Q31" s="1"/>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <v>561</v>
+      </c>
+      <c r="S31">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>5</v>
       </c>
@@ -2573,8 +2634,14 @@
         <v>-1</v>
       </c>
       <c r="Q32" s="1"/>
-    </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <v>581</v>
+      </c>
+      <c r="S32">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>159</v>
       </c>
@@ -2609,8 +2676,14 @@
         <v>0</v>
       </c>
       <c r="Q33" s="1"/>
-    </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <v>601</v>
+      </c>
+      <c r="S33">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>138</v>
       </c>
@@ -2645,8 +2718,14 @@
         <v>0</v>
       </c>
       <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R34">
+        <v>621</v>
+      </c>
+      <c r="S34">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>87</v>
       </c>
@@ -2681,8 +2760,14 @@
         <v>0</v>
       </c>
       <c r="Q35" s="1"/>
-    </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R35">
+        <v>641</v>
+      </c>
+      <c r="S35">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>88</v>
       </c>
@@ -2717,8 +2802,14 @@
         <v>0</v>
       </c>
       <c r="Q36" s="1"/>
-    </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R36">
+        <v>661</v>
+      </c>
+      <c r="S36">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>6</v>
       </c>
@@ -2756,8 +2847,14 @@
         <v>1</v>
       </c>
       <c r="Q37" s="1"/>
-    </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R37">
+        <v>681</v>
+      </c>
+      <c r="S37">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>160</v>
       </c>
@@ -2792,8 +2889,14 @@
         <v>0</v>
       </c>
       <c r="Q38" s="1"/>
-    </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R38">
+        <v>701</v>
+      </c>
+      <c r="S38">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>161</v>
       </c>
@@ -2828,8 +2931,14 @@
         <v>1</v>
       </c>
       <c r="Q39" s="1"/>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R39">
+        <v>721</v>
+      </c>
+      <c r="S39">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>119</v>
       </c>
@@ -2870,8 +2979,14 @@
         <v>0</v>
       </c>
       <c r="Q40" s="1"/>
-    </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R40">
+        <v>741</v>
+      </c>
+      <c r="S40">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>162</v>
       </c>
@@ -2906,8 +3021,14 @@
         <v>0</v>
       </c>
       <c r="Q41" s="1"/>
-    </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R41">
+        <v>761</v>
+      </c>
+      <c r="S41">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>7</v>
       </c>
@@ -2942,8 +3063,14 @@
         <v>0</v>
       </c>
       <c r="Q42" s="1"/>
-    </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R42">
+        <v>781</v>
+      </c>
+      <c r="S42">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>89</v>
       </c>
@@ -2978,8 +3105,14 @@
         <v>0</v>
       </c>
       <c r="Q43" s="1"/>
-    </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>801</v>
+      </c>
+      <c r="S43">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>163</v>
       </c>
@@ -3014,8 +3147,14 @@
         <v>0</v>
       </c>
       <c r="Q44" s="1"/>
-    </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <v>821</v>
+      </c>
+      <c r="S44">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>164</v>
       </c>
@@ -3050,8 +3189,14 @@
         <v>1</v>
       </c>
       <c r="Q45" s="1"/>
-    </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>841</v>
+      </c>
+      <c r="S45">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>49</v>
       </c>
@@ -3086,8 +3231,14 @@
         <v>-1</v>
       </c>
       <c r="Q46" s="1"/>
-    </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>861</v>
+      </c>
+      <c r="S46">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>90</v>
       </c>
@@ -3134,8 +3285,14 @@
         <v>0</v>
       </c>
       <c r="Q47" s="1"/>
-    </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>881</v>
+      </c>
+      <c r="S47">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>139</v>
       </c>
@@ -3170,8 +3327,14 @@
         <v>0</v>
       </c>
       <c r="Q48" s="1"/>
-    </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>901</v>
+      </c>
+      <c r="S48">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="49" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>165</v>
       </c>
@@ -3206,8 +3369,14 @@
         <v>0</v>
       </c>
       <c r="Q49" s="1"/>
-    </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>921</v>
+      </c>
+      <c r="S49">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>166</v>
       </c>
@@ -3242,8 +3411,14 @@
         <v>0</v>
       </c>
       <c r="Q50" s="1"/>
-    </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R50">
+        <v>941</v>
+      </c>
+      <c r="S50">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>140</v>
       </c>
@@ -3278,8 +3453,14 @@
         <v>0</v>
       </c>
       <c r="Q51" s="1"/>
-    </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R51">
+        <v>961</v>
+      </c>
+      <c r="S51">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>167</v>
       </c>
@@ -3314,8 +3495,14 @@
         <v>0</v>
       </c>
       <c r="Q52" s="1"/>
-    </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R52">
+        <v>981</v>
+      </c>
+      <c r="S52">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>141</v>
       </c>
@@ -3350,8 +3537,14 @@
         <v>0</v>
       </c>
       <c r="Q53" s="1"/>
-    </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R53">
+        <v>1001</v>
+      </c>
+      <c r="S53">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="54" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>8</v>
       </c>
@@ -3386,8 +3579,14 @@
         <v>0</v>
       </c>
       <c r="Q54" s="1"/>
-    </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R54">
+        <v>1021</v>
+      </c>
+      <c r="S54">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="55" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>9</v>
       </c>
@@ -3425,8 +3624,14 @@
         <v>0</v>
       </c>
       <c r="Q55" s="1"/>
-    </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R55">
+        <v>1041</v>
+      </c>
+      <c r="S55">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="56" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>122</v>
       </c>
@@ -3461,8 +3666,14 @@
         <v>0</v>
       </c>
       <c r="Q56" s="1"/>
-    </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R56">
+        <v>1061</v>
+      </c>
+      <c r="S56">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="57" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>126</v>
       </c>
@@ -3497,8 +3708,14 @@
         <v>0</v>
       </c>
       <c r="Q57" s="1"/>
-    </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R57">
+        <v>1081</v>
+      </c>
+      <c r="S57">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="58" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>10</v>
       </c>
@@ -3533,8 +3750,14 @@
         <v>0</v>
       </c>
       <c r="Q58" s="1"/>
-    </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R58">
+        <v>1101</v>
+      </c>
+      <c r="S58">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="59" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>11</v>
       </c>
@@ -3575,8 +3798,14 @@
         <v>0</v>
       </c>
       <c r="Q59" s="1"/>
-    </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R59">
+        <v>1121</v>
+      </c>
+      <c r="S59">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="60" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>219</v>
       </c>
@@ -3611,8 +3840,14 @@
         <v>0</v>
       </c>
       <c r="Q60" s="1"/>
-    </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R60">
+        <v>1141</v>
+      </c>
+      <c r="S60">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="61" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>12</v>
       </c>
@@ -3653,8 +3888,14 @@
         <v>0</v>
       </c>
       <c r="Q61" s="1"/>
-    </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R61">
+        <v>1161</v>
+      </c>
+      <c r="S61">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="62" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>168</v>
       </c>
@@ -3689,8 +3930,14 @@
         <v>0</v>
       </c>
       <c r="Q62" s="1"/>
-    </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R62">
+        <v>1181</v>
+      </c>
+      <c r="S62">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="63" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>127</v>
       </c>
@@ -3725,8 +3972,14 @@
         <v>0</v>
       </c>
       <c r="Q63" s="1"/>
-    </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R63">
+        <v>1201</v>
+      </c>
+      <c r="S63">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="64" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>128</v>
       </c>
@@ -3761,8 +4014,14 @@
         <v>0</v>
       </c>
       <c r="Q64" s="1"/>
-    </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R64">
+        <v>1221</v>
+      </c>
+      <c r="S64">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="65" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>169</v>
       </c>
@@ -3797,8 +4056,14 @@
         <v>0</v>
       </c>
       <c r="Q65" s="1"/>
-    </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R65">
+        <v>1241</v>
+      </c>
+      <c r="S65">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="66" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>57</v>
       </c>
@@ -3833,8 +4098,14 @@
         <v>0</v>
       </c>
       <c r="Q66" s="1"/>
-    </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R66">
+        <v>1261</v>
+      </c>
+      <c r="S66">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="67" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>142</v>
       </c>
@@ -3869,8 +4140,14 @@
         <v>0</v>
       </c>
       <c r="Q67" s="1"/>
-    </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R67">
+        <v>1281</v>
+      </c>
+      <c r="S67">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="68" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>170</v>
       </c>
@@ -3905,8 +4182,14 @@
         <v>0</v>
       </c>
       <c r="Q68" s="1"/>
-    </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R68">
+        <v>1301</v>
+      </c>
+      <c r="S68">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="69" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>171</v>
       </c>
@@ -3941,8 +4224,14 @@
         <v>0</v>
       </c>
       <c r="Q69" s="1"/>
-    </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R69">
+        <v>1321</v>
+      </c>
+      <c r="S69">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="70" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>143</v>
       </c>
@@ -3977,8 +4266,14 @@
         <v>0</v>
       </c>
       <c r="Q70" s="1"/>
-    </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R70">
+        <v>1341</v>
+      </c>
+      <c r="S70">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="71" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>13</v>
       </c>
@@ -4022,8 +4317,14 @@
         <v>0</v>
       </c>
       <c r="Q71" s="1"/>
-    </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R71">
+        <v>1361</v>
+      </c>
+      <c r="S71">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="72" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>172</v>
       </c>
@@ -4058,8 +4359,14 @@
         <v>0</v>
       </c>
       <c r="Q72" s="1"/>
-    </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R72">
+        <v>1381</v>
+      </c>
+      <c r="S72">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="73" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>14</v>
       </c>
@@ -4097,8 +4404,14 @@
         <v>1</v>
       </c>
       <c r="Q73" s="1"/>
-    </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R73">
+        <v>1401</v>
+      </c>
+      <c r="S73">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="74" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>173</v>
       </c>
@@ -4133,8 +4446,14 @@
         <v>0</v>
       </c>
       <c r="Q74" s="1"/>
-    </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R74">
+        <v>1421</v>
+      </c>
+      <c r="S74">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="75" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>113</v>
       </c>
@@ -4169,8 +4488,14 @@
         <v>0</v>
       </c>
       <c r="Q75" s="1"/>
-    </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R75">
+        <v>1441</v>
+      </c>
+      <c r="S75">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="76" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>15</v>
       </c>
@@ -4205,8 +4530,14 @@
         <v>0</v>
       </c>
       <c r="Q76" s="1"/>
-    </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R76">
+        <v>1461</v>
+      </c>
+      <c r="S76">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="77" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>16</v>
       </c>
@@ -4247,8 +4578,14 @@
         <v>0</v>
       </c>
       <c r="Q77" s="1"/>
-    </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R77">
+        <v>1481</v>
+      </c>
+      <c r="S77">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="78" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>220</v>
       </c>
@@ -4283,8 +4620,14 @@
         <v>1</v>
       </c>
       <c r="Q78" s="1"/>
-    </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R78">
+        <v>1501</v>
+      </c>
+      <c r="S78">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="79" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>17</v>
       </c>
@@ -4319,8 +4662,14 @@
         <v>0</v>
       </c>
       <c r="Q79" s="1"/>
-    </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R79">
+        <v>1521</v>
+      </c>
+      <c r="S79">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="80" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>174</v>
       </c>
@@ -4355,8 +4704,14 @@
         <v>0</v>
       </c>
       <c r="Q80" s="1"/>
-    </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R80">
+        <v>1541</v>
+      </c>
+      <c r="S80">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="81" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>175</v>
       </c>
@@ -4391,8 +4746,14 @@
         <v>1</v>
       </c>
       <c r="Q81" s="1"/>
-    </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R81">
+        <v>1561</v>
+      </c>
+      <c r="S81">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="82" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>176</v>
       </c>
@@ -4427,8 +4788,14 @@
         <v>0</v>
       </c>
       <c r="Q82" s="1"/>
-    </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R82">
+        <v>1581</v>
+      </c>
+      <c r="S82">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="83" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>58</v>
       </c>
@@ -4463,8 +4830,14 @@
         <v>0</v>
       </c>
       <c r="Q83" s="1"/>
-    </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R83">
+        <v>1601</v>
+      </c>
+      <c r="S83">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="84" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>18</v>
       </c>
@@ -4511,8 +4884,14 @@
         <v>0</v>
       </c>
       <c r="Q84" s="1"/>
-    </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R84">
+        <v>1621</v>
+      </c>
+      <c r="S84">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="85" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>221</v>
       </c>
@@ -4547,8 +4926,14 @@
         <v>1</v>
       </c>
       <c r="Q85" s="1"/>
-    </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R85">
+        <v>1641</v>
+      </c>
+      <c r="S85">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="86" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>222</v>
       </c>
@@ -4583,8 +4968,14 @@
         <v>0</v>
       </c>
       <c r="Q86" s="1"/>
-    </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R86">
+        <v>1661</v>
+      </c>
+      <c r="S86">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="87" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>129</v>
       </c>
@@ -4619,8 +5010,14 @@
         <v>0</v>
       </c>
       <c r="Q87" s="1"/>
-    </row>
-    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R87">
+        <v>1681</v>
+      </c>
+      <c r="S87">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="88" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>19</v>
       </c>
@@ -4661,8 +5058,14 @@
         <v>0</v>
       </c>
       <c r="Q88" s="1"/>
-    </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R88">
+        <v>1701</v>
+      </c>
+      <c r="S88">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="89" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>144</v>
       </c>
@@ -4697,8 +5100,14 @@
         <v>0</v>
       </c>
       <c r="Q89" s="1"/>
-    </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R89">
+        <v>1721</v>
+      </c>
+      <c r="S89">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="90" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>177</v>
       </c>
@@ -4733,8 +5142,14 @@
         <v>0</v>
       </c>
       <c r="Q90" s="1"/>
-    </row>
-    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R90">
+        <v>1741</v>
+      </c>
+      <c r="S90">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="91" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>178</v>
       </c>
@@ -4769,8 +5184,14 @@
         <v>1</v>
       </c>
       <c r="Q91" s="1"/>
-    </row>
-    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R91">
+        <v>1761</v>
+      </c>
+      <c r="S91">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="92" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>145</v>
       </c>
@@ -4805,8 +5226,14 @@
         <v>0</v>
       </c>
       <c r="Q92" s="1"/>
-    </row>
-    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R92">
+        <v>1781</v>
+      </c>
+      <c r="S92">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="93" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>130</v>
       </c>
@@ -4841,8 +5268,14 @@
         <v>0</v>
       </c>
       <c r="Q93" s="1"/>
-    </row>
-    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R93">
+        <v>1801</v>
+      </c>
+      <c r="S93">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="94" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>223</v>
       </c>
@@ -4877,8 +5310,14 @@
         <v>0</v>
       </c>
       <c r="Q94" s="1"/>
-    </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R94">
+        <v>1821</v>
+      </c>
+      <c r="S94">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="95" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>59</v>
       </c>
@@ -4913,8 +5352,14 @@
         <v>0</v>
       </c>
       <c r="Q95" s="1"/>
-    </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R95">
+        <v>1841</v>
+      </c>
+      <c r="S95">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="96" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>224</v>
       </c>
@@ -4952,8 +5397,14 @@
         <v>0</v>
       </c>
       <c r="Q96" s="1"/>
-    </row>
-    <row r="97" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R96">
+        <v>1861</v>
+      </c>
+      <c r="S96">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="97" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>91</v>
       </c>
@@ -4994,8 +5445,14 @@
         <v>0</v>
       </c>
       <c r="Q97" s="1"/>
-    </row>
-    <row r="98" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R97">
+        <v>1881</v>
+      </c>
+      <c r="S97">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="98" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>25</v>
       </c>
@@ -5030,8 +5487,14 @@
         <v>0</v>
       </c>
       <c r="Q98" s="1"/>
-    </row>
-    <row r="99" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R98">
+        <v>1901</v>
+      </c>
+      <c r="S98">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="99" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>20</v>
       </c>
@@ -5072,8 +5535,14 @@
         <v>0</v>
       </c>
       <c r="Q99" s="1"/>
-    </row>
-    <row r="100" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R99">
+        <v>1921</v>
+      </c>
+      <c r="S99">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="100" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>146</v>
       </c>
@@ -5108,8 +5577,14 @@
         <v>0</v>
       </c>
       <c r="Q100" s="1"/>
-    </row>
-    <row r="101" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R100">
+        <v>1941</v>
+      </c>
+      <c r="S100">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="101" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>225</v>
       </c>
@@ -5144,8 +5619,14 @@
         <v>1</v>
       </c>
       <c r="Q101" s="1"/>
-    </row>
-    <row r="102" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R101">
+        <v>1961</v>
+      </c>
+      <c r="S101">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="102" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>226</v>
       </c>
@@ -5180,8 +5661,14 @@
         <v>1</v>
       </c>
       <c r="Q102" s="1"/>
-    </row>
-    <row r="103" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R102">
+        <v>1981</v>
+      </c>
+      <c r="S102">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="103" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>21</v>
       </c>
@@ -5222,8 +5709,14 @@
         <v>0</v>
       </c>
       <c r="Q103" s="1"/>
-    </row>
-    <row r="104" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R103">
+        <v>2001</v>
+      </c>
+      <c r="S103">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="104" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>22</v>
       </c>
@@ -5264,8 +5757,14 @@
         <v>0</v>
       </c>
       <c r="Q104" s="1"/>
-    </row>
-    <row r="105" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R104">
+        <v>2021</v>
+      </c>
+      <c r="S104">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="105" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>92</v>
       </c>
@@ -5300,8 +5799,14 @@
         <v>0</v>
       </c>
       <c r="Q105" s="1"/>
-    </row>
-    <row r="106" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R105">
+        <v>2041</v>
+      </c>
+      <c r="S105">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="106" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>23</v>
       </c>
@@ -5336,8 +5841,14 @@
         <v>0</v>
       </c>
       <c r="Q106" s="1"/>
-    </row>
-    <row r="107" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R106">
+        <v>2061</v>
+      </c>
+      <c r="S106">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="107" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>60</v>
       </c>
@@ -5372,8 +5883,14 @@
         <v>0</v>
       </c>
       <c r="Q107" s="1"/>
-    </row>
-    <row r="108" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R107">
+        <v>2081</v>
+      </c>
+      <c r="S107">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="108" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>227</v>
       </c>
@@ -5408,8 +5925,14 @@
         <v>1</v>
       </c>
       <c r="Q108" s="1"/>
-    </row>
-    <row r="109" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R108">
+        <v>2101</v>
+      </c>
+      <c r="S108">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="109" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>61</v>
       </c>
@@ -5444,8 +5967,14 @@
         <v>0</v>
       </c>
       <c r="Q109" s="1"/>
-    </row>
-    <row r="110" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R109">
+        <v>2121</v>
+      </c>
+      <c r="S109">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="110" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>24</v>
       </c>
@@ -5486,8 +6015,14 @@
         <v>0</v>
       </c>
       <c r="Q110" s="1"/>
-    </row>
-    <row r="111" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R110">
+        <v>2141</v>
+      </c>
+      <c r="S110">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="111" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>131</v>
       </c>
@@ -5522,8 +6057,14 @@
         <v>0</v>
       </c>
       <c r="Q111" s="1"/>
-    </row>
-    <row r="112" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R111">
+        <v>2161</v>
+      </c>
+      <c r="S111">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="112" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>62</v>
       </c>
@@ -5564,8 +6105,14 @@
         <v>0</v>
       </c>
       <c r="Q112" s="1"/>
-    </row>
-    <row r="113" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R112">
+        <v>2181</v>
+      </c>
+      <c r="S112">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="113" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>63</v>
       </c>
@@ -5600,8 +6147,14 @@
         <v>0</v>
       </c>
       <c r="Q113" s="1"/>
-    </row>
-    <row r="114" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R113">
+        <v>2201</v>
+      </c>
+      <c r="S113">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="114" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>228</v>
       </c>
@@ -5636,8 +6189,14 @@
         <v>0</v>
       </c>
       <c r="Q114" s="1"/>
-    </row>
-    <row r="115" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R114">
+        <v>2221</v>
+      </c>
+      <c r="S114">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="115" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>93</v>
       </c>
@@ -5672,8 +6231,14 @@
         <v>1</v>
       </c>
       <c r="Q115" s="1"/>
-    </row>
-    <row r="116" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R115">
+        <v>2241</v>
+      </c>
+      <c r="S115">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="116" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>94</v>
       </c>
@@ -5708,8 +6273,14 @@
         <v>0</v>
       </c>
       <c r="Q116" s="1"/>
-    </row>
-    <row r="117" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R116">
+        <v>2261</v>
+      </c>
+      <c r="S116">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="117" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>64</v>
       </c>
@@ -5750,8 +6321,14 @@
         <v>0</v>
       </c>
       <c r="Q117" s="1"/>
-    </row>
-    <row r="118" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R117">
+        <v>2281</v>
+      </c>
+      <c r="S117">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="118" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>179</v>
       </c>
@@ -5786,8 +6363,14 @@
         <v>1</v>
       </c>
       <c r="Q118" s="1"/>
-    </row>
-    <row r="119" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R118">
+        <v>2301</v>
+      </c>
+      <c r="S118">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="119" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>95</v>
       </c>
@@ -5822,8 +6405,14 @@
         <v>0</v>
       </c>
       <c r="Q119" s="1"/>
-    </row>
-    <row r="120" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R119">
+        <v>2321</v>
+      </c>
+      <c r="S119">
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="120" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>26</v>
       </c>
@@ -5858,8 +6447,14 @@
         <v>0</v>
       </c>
       <c r="Q120" s="1"/>
-    </row>
-    <row r="121" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R120">
+        <v>2341</v>
+      </c>
+      <c r="S120">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="121" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>229</v>
       </c>
@@ -5894,8 +6489,14 @@
         <v>0</v>
       </c>
       <c r="Q121" s="1"/>
-    </row>
-    <row r="122" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R121">
+        <v>2361</v>
+      </c>
+      <c r="S121">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="122" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>65</v>
       </c>
@@ -5930,8 +6531,14 @@
         <v>0</v>
       </c>
       <c r="Q122" s="1"/>
-    </row>
-    <row r="123" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R122">
+        <v>2381</v>
+      </c>
+      <c r="S122">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="123" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>66</v>
       </c>
@@ -5972,8 +6579,14 @@
         <v>0</v>
       </c>
       <c r="Q123" s="1"/>
-    </row>
-    <row r="124" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R123">
+        <v>2401</v>
+      </c>
+      <c r="S123">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="124" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>96</v>
       </c>
@@ -6008,8 +6621,14 @@
         <v>0</v>
       </c>
       <c r="Q124" s="1"/>
-    </row>
-    <row r="125" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R124">
+        <v>2421</v>
+      </c>
+      <c r="S124">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="125" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>27</v>
       </c>
@@ -6047,8 +6666,14 @@
         <v>1</v>
       </c>
       <c r="Q125" s="1"/>
-    </row>
-    <row r="126" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R125">
+        <v>2441</v>
+      </c>
+      <c r="S125">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="126" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>180</v>
       </c>
@@ -6083,8 +6708,14 @@
         <v>-1</v>
       </c>
       <c r="Q126" s="1"/>
-    </row>
-    <row r="127" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R126">
+        <v>2461</v>
+      </c>
+      <c r="S126">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="127" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>67</v>
       </c>
@@ -6119,8 +6750,14 @@
         <v>0</v>
       </c>
       <c r="Q127" s="1"/>
-    </row>
-    <row r="128" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R127">
+        <v>2481</v>
+      </c>
+      <c r="S127">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="128" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>181</v>
       </c>
@@ -6155,8 +6792,14 @@
         <v>0</v>
       </c>
       <c r="Q128" s="1"/>
-    </row>
-    <row r="129" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R128">
+        <v>2501</v>
+      </c>
+      <c r="S128">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="129" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>182</v>
       </c>
@@ -6191,8 +6834,14 @@
         <v>-1</v>
       </c>
       <c r="Q129" s="1"/>
-    </row>
-    <row r="130" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R129">
+        <v>2521</v>
+      </c>
+      <c r="S129">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="130" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>28</v>
       </c>
@@ -6230,8 +6879,14 @@
         <v>1</v>
       </c>
       <c r="Q130" s="1"/>
-    </row>
-    <row r="131" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R130">
+        <v>2541</v>
+      </c>
+      <c r="S130">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="131" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>231</v>
       </c>
@@ -6266,8 +6921,14 @@
         <v>0</v>
       </c>
       <c r="Q131" s="1"/>
-    </row>
-    <row r="132" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R131">
+        <v>2561</v>
+      </c>
+      <c r="S131">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="132" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>68</v>
       </c>
@@ -6302,8 +6963,14 @@
         <v>0</v>
       </c>
       <c r="Q132" s="1"/>
-    </row>
-    <row r="133" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R132">
+        <v>2581</v>
+      </c>
+      <c r="S132">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="133" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>230</v>
       </c>
@@ -6338,8 +7005,14 @@
         <v>0</v>
       </c>
       <c r="Q133" s="1"/>
-    </row>
-    <row r="134" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R133">
+        <v>2601</v>
+      </c>
+      <c r="S133">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="134" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>29</v>
       </c>
@@ -6380,8 +7053,14 @@
         <v>0</v>
       </c>
       <c r="Q134" s="1"/>
-    </row>
-    <row r="135" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R134">
+        <v>2621</v>
+      </c>
+      <c r="S134">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="135" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>183</v>
       </c>
@@ -6416,8 +7095,14 @@
         <v>1</v>
       </c>
       <c r="Q135" s="1"/>
-    </row>
-    <row r="136" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R135">
+        <v>2641</v>
+      </c>
+      <c r="S135">
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="136" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>184</v>
       </c>
@@ -6452,8 +7137,14 @@
         <v>0</v>
       </c>
       <c r="Q136" s="1"/>
-    </row>
-    <row r="137" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R136">
+        <v>2661</v>
+      </c>
+      <c r="S136">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="137" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>185</v>
       </c>
@@ -6488,8 +7179,14 @@
         <v>1</v>
       </c>
       <c r="Q137" s="1"/>
-    </row>
-    <row r="138" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R137">
+        <v>2681</v>
+      </c>
+      <c r="S137">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="138" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>97</v>
       </c>
@@ -6524,8 +7221,14 @@
         <v>0</v>
       </c>
       <c r="Q138" s="1"/>
-    </row>
-    <row r="139" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R138">
+        <v>2701</v>
+      </c>
+      <c r="S138">
+        <v>2720</v>
+      </c>
+    </row>
+    <row r="139" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>120</v>
       </c>
@@ -6560,8 +7263,14 @@
         <v>-1</v>
       </c>
       <c r="Q139" s="1"/>
-    </row>
-    <row r="140" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R139">
+        <v>2721</v>
+      </c>
+      <c r="S139">
+        <v>2740</v>
+      </c>
+    </row>
+    <row r="140" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>114</v>
       </c>
@@ -6596,8 +7305,14 @@
         <v>0</v>
       </c>
       <c r="Q140" s="1"/>
-    </row>
-    <row r="141" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R140">
+        <v>2741</v>
+      </c>
+      <c r="S140">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="141" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>232</v>
       </c>
@@ -6632,8 +7347,14 @@
         <v>0</v>
       </c>
       <c r="Q141" s="1"/>
-    </row>
-    <row r="142" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R141">
+        <v>2761</v>
+      </c>
+      <c r="S141">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="142" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>98</v>
       </c>
@@ -6668,8 +7389,14 @@
         <v>0</v>
       </c>
       <c r="Q142" s="1"/>
-    </row>
-    <row r="143" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R142">
+        <v>2781</v>
+      </c>
+      <c r="S142">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="143" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>30</v>
       </c>
@@ -6704,8 +7431,14 @@
         <v>0</v>
       </c>
       <c r="Q143" s="1"/>
-    </row>
-    <row r="144" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R143">
+        <v>2801</v>
+      </c>
+      <c r="S143">
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="144" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>186</v>
       </c>
@@ -6740,8 +7473,14 @@
         <v>0</v>
       </c>
       <c r="Q144" s="1"/>
-    </row>
-    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R144">
+        <v>2821</v>
+      </c>
+      <c r="S144">
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="145" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>31</v>
       </c>
@@ -6776,8 +7515,14 @@
         <v>0</v>
       </c>
       <c r="Q145" s="1"/>
-    </row>
-    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R145">
+        <v>2841</v>
+      </c>
+      <c r="S145">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="146" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>32</v>
       </c>
@@ -6812,8 +7557,14 @@
         <v>0</v>
       </c>
       <c r="Q146" s="1"/>
-    </row>
-    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R146">
+        <v>2861</v>
+      </c>
+      <c r="S146">
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="147" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>99</v>
       </c>
@@ -6848,8 +7599,14 @@
         <v>0</v>
       </c>
       <c r="Q147" s="1"/>
-    </row>
-    <row r="148" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R147">
+        <v>2881</v>
+      </c>
+      <c r="S147">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="148" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>187</v>
       </c>
@@ -6884,8 +7641,14 @@
         <v>0</v>
       </c>
       <c r="Q148" s="1"/>
-    </row>
-    <row r="149" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R148">
+        <v>2901</v>
+      </c>
+      <c r="S148">
+        <v>2920</v>
+      </c>
+    </row>
+    <row r="149" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>188</v>
       </c>
@@ -6920,8 +7683,14 @@
         <v>0</v>
       </c>
       <c r="Q149" s="1"/>
-    </row>
-    <row r="150" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R149">
+        <v>2921</v>
+      </c>
+      <c r="S149">
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="150" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>189</v>
       </c>
@@ -6956,8 +7725,14 @@
         <v>0</v>
       </c>
       <c r="Q150" s="1"/>
-    </row>
-    <row r="151" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R150">
+        <v>2941</v>
+      </c>
+      <c r="S150">
+        <v>2960</v>
+      </c>
+    </row>
+    <row r="151" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>190</v>
       </c>
@@ -6992,8 +7767,14 @@
         <v>0</v>
       </c>
       <c r="Q151" s="1"/>
-    </row>
-    <row r="152" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R151">
+        <v>2961</v>
+      </c>
+      <c r="S151">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="152" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>33</v>
       </c>
@@ -7028,8 +7809,14 @@
         <v>0</v>
       </c>
       <c r="Q152" s="1"/>
-    </row>
-    <row r="153" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R152">
+        <v>2981</v>
+      </c>
+      <c r="S152">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="153" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>69</v>
       </c>
@@ -7064,8 +7851,14 @@
         <v>0</v>
       </c>
       <c r="Q153" s="1"/>
-    </row>
-    <row r="154" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R153">
+        <v>3001</v>
+      </c>
+      <c r="S153">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="154" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>100</v>
       </c>
@@ -7100,8 +7893,14 @@
         <v>0</v>
       </c>
       <c r="Q154" s="1"/>
-    </row>
-    <row r="155" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R154">
+        <v>3021</v>
+      </c>
+      <c r="S154">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="155" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>191</v>
       </c>
@@ -7136,8 +7935,14 @@
         <v>0</v>
       </c>
       <c r="Q155" s="1"/>
-    </row>
-    <row r="156" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R155">
+        <v>3041</v>
+      </c>
+      <c r="S155">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="156" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>147</v>
       </c>
@@ -7172,8 +7977,14 @@
         <v>1</v>
       </c>
       <c r="Q156" s="1"/>
-    </row>
-    <row r="157" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R156">
+        <v>3061</v>
+      </c>
+      <c r="S156">
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="157" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>192</v>
       </c>
@@ -7208,8 +8019,14 @@
         <v>0</v>
       </c>
       <c r="Q157" s="1"/>
-    </row>
-    <row r="158" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R157">
+        <v>3081</v>
+      </c>
+      <c r="S157">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="158" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>101</v>
       </c>
@@ -7244,8 +8061,14 @@
         <v>0</v>
       </c>
       <c r="Q158" s="1"/>
-    </row>
-    <row r="159" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R158">
+        <v>3101</v>
+      </c>
+      <c r="S158">
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="159" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>70</v>
       </c>
@@ -7286,8 +8109,14 @@
         <v>0</v>
       </c>
       <c r="Q159" s="1"/>
-    </row>
-    <row r="160" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R159">
+        <v>3121</v>
+      </c>
+      <c r="S159">
+        <v>3140</v>
+      </c>
+    </row>
+    <row r="160" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>34</v>
       </c>
@@ -7328,8 +8157,14 @@
         <v>0</v>
       </c>
       <c r="Q160" s="1"/>
-    </row>
-    <row r="161" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R160">
+        <v>3141</v>
+      </c>
+      <c r="S160">
+        <v>3160</v>
+      </c>
+    </row>
+    <row r="161" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>233</v>
       </c>
@@ -7364,8 +8199,14 @@
         <v>1</v>
       </c>
       <c r="Q161" s="1"/>
-    </row>
-    <row r="162" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R161">
+        <v>3161</v>
+      </c>
+      <c r="S161">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="162" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>234</v>
       </c>
@@ -7400,8 +8241,14 @@
         <v>1</v>
       </c>
       <c r="Q162" s="1"/>
-    </row>
-    <row r="163" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R162">
+        <v>3181</v>
+      </c>
+      <c r="S162">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="163" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>115</v>
       </c>
@@ -7436,8 +8283,14 @@
         <v>0</v>
       </c>
       <c r="Q163" s="1"/>
-    </row>
-    <row r="164" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R163">
+        <v>3201</v>
+      </c>
+      <c r="S163">
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="164" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>71</v>
       </c>
@@ -7472,8 +8325,14 @@
         <v>1</v>
       </c>
       <c r="Q164" s="1"/>
-    </row>
-    <row r="165" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R164">
+        <v>3221</v>
+      </c>
+      <c r="S164">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="165" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>72</v>
       </c>
@@ -7508,8 +8367,14 @@
         <v>0</v>
       </c>
       <c r="Q165" s="1"/>
-    </row>
-    <row r="166" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R165">
+        <v>3241</v>
+      </c>
+      <c r="S165">
+        <v>3260</v>
+      </c>
+    </row>
+    <row r="166" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>73</v>
       </c>
@@ -7544,8 +8409,14 @@
         <v>0</v>
       </c>
       <c r="Q166" s="1"/>
-    </row>
-    <row r="167" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R166">
+        <v>3261</v>
+      </c>
+      <c r="S166">
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="167" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>148</v>
       </c>
@@ -7580,8 +8451,14 @@
         <v>0</v>
       </c>
       <c r="Q167" s="1"/>
-    </row>
-    <row r="168" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R167">
+        <v>3281</v>
+      </c>
+      <c r="S167">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="168" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>116</v>
       </c>
@@ -7616,8 +8493,14 @@
         <v>0</v>
       </c>
       <c r="Q168" s="1"/>
-    </row>
-    <row r="169" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R168">
+        <v>3301</v>
+      </c>
+      <c r="S168">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="169" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>149</v>
       </c>
@@ -7652,8 +8535,14 @@
         <v>0</v>
       </c>
       <c r="Q169" s="1"/>
-    </row>
-    <row r="170" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R169">
+        <v>3321</v>
+      </c>
+      <c r="S169">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="170" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>150</v>
       </c>
@@ -7688,8 +8577,14 @@
         <v>0</v>
       </c>
       <c r="Q170" s="1"/>
-    </row>
-    <row r="171" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R170">
+        <v>3341</v>
+      </c>
+      <c r="S170">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="171" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>74</v>
       </c>
@@ -7730,8 +8625,14 @@
         <v>1</v>
       </c>
       <c r="Q171" s="1"/>
-    </row>
-    <row r="172" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R171">
+        <v>3361</v>
+      </c>
+      <c r="S171">
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="172" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>102</v>
       </c>
@@ -7766,8 +8667,14 @@
         <v>0</v>
       </c>
       <c r="Q172" s="1"/>
-    </row>
-    <row r="173" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R172">
+        <v>3381</v>
+      </c>
+      <c r="S172">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="173" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>235</v>
       </c>
@@ -7802,8 +8709,14 @@
         <v>0</v>
       </c>
       <c r="Q173" s="1"/>
-    </row>
-    <row r="174" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R173">
+        <v>3401</v>
+      </c>
+      <c r="S173">
+        <v>3420</v>
+      </c>
+    </row>
+    <row r="174" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>117</v>
       </c>
@@ -7838,8 +8751,14 @@
         <v>0</v>
       </c>
       <c r="Q174" s="1"/>
-    </row>
-    <row r="175" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R174">
+        <v>3421</v>
+      </c>
+      <c r="S174">
+        <v>3440</v>
+      </c>
+    </row>
+    <row r="175" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>236</v>
       </c>
@@ -7874,8 +8793,14 @@
         <v>0</v>
       </c>
       <c r="Q175" s="1"/>
-    </row>
-    <row r="176" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R175">
+        <v>3441</v>
+      </c>
+      <c r="S175">
+        <v>3460</v>
+      </c>
+    </row>
+    <row r="176" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>35</v>
       </c>
@@ -7916,8 +8841,14 @@
         <v>0</v>
       </c>
       <c r="Q176" s="1"/>
-    </row>
-    <row r="177" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R176">
+        <v>3461</v>
+      </c>
+      <c r="S176">
+        <v>3480</v>
+      </c>
+    </row>
+    <row r="177" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>36</v>
       </c>
@@ -7958,8 +8889,14 @@
         <v>0</v>
       </c>
       <c r="Q177" s="1"/>
-    </row>
-    <row r="178" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R177">
+        <v>3481</v>
+      </c>
+      <c r="S177">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="178" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>151</v>
       </c>
@@ -7994,8 +8931,14 @@
         <v>0</v>
       </c>
       <c r="Q178" s="1"/>
-    </row>
-    <row r="179" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R178">
+        <v>3501</v>
+      </c>
+      <c r="S178">
+        <v>3520</v>
+      </c>
+    </row>
+    <row r="179" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>237</v>
       </c>
@@ -8030,8 +8973,14 @@
         <v>0</v>
       </c>
       <c r="Q179" s="1"/>
-    </row>
-    <row r="180" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R179">
+        <v>3521</v>
+      </c>
+      <c r="S179">
+        <v>3540</v>
+      </c>
+    </row>
+    <row r="180" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>75</v>
       </c>
@@ -8066,8 +9015,14 @@
         <v>0</v>
       </c>
       <c r="Q180" s="1"/>
-    </row>
-    <row r="181" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R180">
+        <v>3541</v>
+      </c>
+      <c r="S180">
+        <v>3560</v>
+      </c>
+    </row>
+    <row r="181" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>76</v>
       </c>
@@ -8102,8 +9057,14 @@
         <v>0</v>
       </c>
       <c r="Q181" s="1"/>
-    </row>
-    <row r="182" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R181">
+        <v>3561</v>
+      </c>
+      <c r="S181">
+        <v>3580</v>
+      </c>
+    </row>
+    <row r="182" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>250</v>
       </c>
@@ -8138,8 +9099,14 @@
         <v>0</v>
       </c>
       <c r="Q182" s="1"/>
-    </row>
-    <row r="183" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R182">
+        <v>3581</v>
+      </c>
+      <c r="S182">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="183" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>103</v>
       </c>
@@ -8177,8 +9144,14 @@
         <v>0</v>
       </c>
       <c r="Q183" s="1"/>
-    </row>
-    <row r="184" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R183">
+        <v>3601</v>
+      </c>
+      <c r="S183">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="184" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>238</v>
       </c>
@@ -8213,8 +9186,14 @@
         <v>0</v>
       </c>
       <c r="Q184" s="1"/>
-    </row>
-    <row r="185" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R184">
+        <v>3621</v>
+      </c>
+      <c r="S184">
+        <v>3640</v>
+      </c>
+    </row>
+    <row r="185" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>239</v>
       </c>
@@ -8249,8 +9228,14 @@
         <v>1</v>
       </c>
       <c r="Q185" s="1"/>
-    </row>
-    <row r="186" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R185">
+        <v>3641</v>
+      </c>
+      <c r="S185">
+        <v>3660</v>
+      </c>
+    </row>
+    <row r="186" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>37</v>
       </c>
@@ -8288,8 +9273,14 @@
         <v>0</v>
       </c>
       <c r="Q186" s="1"/>
-    </row>
-    <row r="187" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R186">
+        <v>3661</v>
+      </c>
+      <c r="S186">
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="187" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>193</v>
       </c>
@@ -8324,8 +9315,14 @@
         <v>0</v>
       </c>
       <c r="Q187" s="1"/>
-    </row>
-    <row r="188" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R187">
+        <v>3681</v>
+      </c>
+      <c r="S187">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="188" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>194</v>
       </c>
@@ -8360,8 +9357,14 @@
         <v>0</v>
       </c>
       <c r="Q188" s="1"/>
-    </row>
-    <row r="189" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R188">
+        <v>3701</v>
+      </c>
+      <c r="S188">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="189" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>195</v>
       </c>
@@ -8396,8 +9399,14 @@
         <v>0</v>
       </c>
       <c r="Q189" s="1"/>
-    </row>
-    <row r="190" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R189">
+        <v>3721</v>
+      </c>
+      <c r="S189">
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="190" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>77</v>
       </c>
@@ -8444,8 +9453,14 @@
         <v>1</v>
       </c>
       <c r="Q190" s="1"/>
-    </row>
-    <row r="191" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R190">
+        <v>3741</v>
+      </c>
+      <c r="S190">
+        <v>3760</v>
+      </c>
+    </row>
+    <row r="191" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>38</v>
       </c>
@@ -8480,8 +9495,14 @@
         <v>0</v>
       </c>
       <c r="Q191" s="1"/>
-    </row>
-    <row r="192" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R191">
+        <v>3761</v>
+      </c>
+      <c r="S191">
+        <v>3780</v>
+      </c>
+    </row>
+    <row r="192" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>39</v>
       </c>
@@ -8516,8 +9537,14 @@
         <v>0</v>
       </c>
       <c r="Q192" s="1"/>
-    </row>
-    <row r="193" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R192">
+        <v>3781</v>
+      </c>
+      <c r="S192">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="193" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>241</v>
       </c>
@@ -8552,8 +9579,14 @@
         <v>0</v>
       </c>
       <c r="Q193" s="1"/>
-    </row>
-    <row r="194" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R193">
+        <v>3801</v>
+      </c>
+      <c r="S193">
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="194" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>196</v>
       </c>
@@ -8588,8 +9621,14 @@
         <v>1</v>
       </c>
       <c r="Q194" s="1"/>
-    </row>
-    <row r="195" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R194">
+        <v>3821</v>
+      </c>
+      <c r="S194">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="195" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>40</v>
       </c>
@@ -8624,8 +9663,14 @@
         <v>-1</v>
       </c>
       <c r="Q195" s="1"/>
-    </row>
-    <row r="196" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R195">
+        <v>3841</v>
+      </c>
+      <c r="S195">
+        <v>3860</v>
+      </c>
+    </row>
+    <row r="196" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>197</v>
       </c>
@@ -8660,8 +9705,14 @@
         <v>0</v>
       </c>
       <c r="Q196" s="1"/>
-    </row>
-    <row r="197" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R196">
+        <v>3861</v>
+      </c>
+      <c r="S196">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="197" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>198</v>
       </c>
@@ -8696,8 +9747,14 @@
         <v>0</v>
       </c>
       <c r="Q197" s="1"/>
-    </row>
-    <row r="198" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R197">
+        <v>3881</v>
+      </c>
+      <c r="S197">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="198" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>240</v>
       </c>
@@ -8732,8 +9789,14 @@
         <v>1</v>
       </c>
       <c r="Q198" s="1"/>
-    </row>
-    <row r="199" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R198">
+        <v>3901</v>
+      </c>
+      <c r="S198">
+        <v>3920</v>
+      </c>
+    </row>
+    <row r="199" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>104</v>
       </c>
@@ -8768,8 +9831,14 @@
         <v>0</v>
       </c>
       <c r="Q199" s="1"/>
-    </row>
-    <row r="200" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R199">
+        <v>3921</v>
+      </c>
+      <c r="S199">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="200" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>265</v>
       </c>
@@ -8804,8 +9873,14 @@
         <v>0</v>
       </c>
       <c r="Q200" s="1"/>
-    </row>
-    <row r="201" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R200">
+        <v>3941</v>
+      </c>
+      <c r="S200">
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="201" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>199</v>
       </c>
@@ -8840,8 +9915,14 @@
         <v>0</v>
       </c>
       <c r="Q201" s="1"/>
-    </row>
-    <row r="202" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R201">
+        <v>3961</v>
+      </c>
+      <c r="S201">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="202" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>105</v>
       </c>
@@ -8876,8 +9957,14 @@
         <v>0</v>
       </c>
       <c r="Q202" s="1"/>
-    </row>
-    <row r="203" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R202">
+        <v>3981</v>
+      </c>
+      <c r="S202">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="203" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
         <v>41</v>
       </c>
@@ -8915,8 +10002,14 @@
         <v>1</v>
       </c>
       <c r="Q203" s="1"/>
-    </row>
-    <row r="204" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R203">
+        <v>4001</v>
+      </c>
+      <c r="S203">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="204" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
         <v>42</v>
       </c>
@@ -8954,8 +10047,14 @@
         <v>1</v>
       </c>
       <c r="Q204" s="1"/>
-    </row>
-    <row r="205" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R204">
+        <v>4021</v>
+      </c>
+      <c r="S204">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="205" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>200</v>
       </c>
@@ -8990,8 +10089,14 @@
         <v>0</v>
       </c>
       <c r="Q205" s="1"/>
-    </row>
-    <row r="206" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R205">
+        <v>4041</v>
+      </c>
+      <c r="S205">
+        <v>4060</v>
+      </c>
+    </row>
+    <row r="206" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>242</v>
       </c>
@@ -9026,8 +10131,14 @@
         <v>0</v>
       </c>
       <c r="Q206" s="1"/>
-    </row>
-    <row r="207" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R206">
+        <v>4061</v>
+      </c>
+      <c r="S206">
+        <v>4080</v>
+      </c>
+    </row>
+    <row r="207" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>118</v>
       </c>
@@ -9062,8 +10173,14 @@
         <v>0</v>
       </c>
       <c r="Q207" s="1"/>
-    </row>
-    <row r="208" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R207">
+        <v>4081</v>
+      </c>
+      <c r="S207">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="208" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>201</v>
       </c>
@@ -9098,8 +10215,14 @@
         <v>-1</v>
       </c>
       <c r="Q208" s="1"/>
-    </row>
-    <row r="209" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R208">
+        <v>4101</v>
+      </c>
+      <c r="S208">
+        <v>4120</v>
+      </c>
+    </row>
+    <row r="209" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>243</v>
       </c>
@@ -9134,8 +10257,14 @@
         <v>0</v>
       </c>
       <c r="Q209" s="1"/>
-    </row>
-    <row r="210" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R209">
+        <v>4121</v>
+      </c>
+      <c r="S209">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="210" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>43</v>
       </c>
@@ -9182,8 +10311,14 @@
         <v>1</v>
       </c>
       <c r="Q210" s="1"/>
-    </row>
-    <row r="211" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R210">
+        <v>4141</v>
+      </c>
+      <c r="S210">
+        <v>4160</v>
+      </c>
+    </row>
+    <row r="211" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>44</v>
       </c>
@@ -9224,8 +10359,14 @@
         <v>0</v>
       </c>
       <c r="Q211" s="1"/>
-    </row>
-    <row r="212" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R211">
+        <v>4161</v>
+      </c>
+      <c r="S211">
+        <v>4180</v>
+      </c>
+    </row>
+    <row r="212" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>244</v>
       </c>
@@ -9260,8 +10401,14 @@
         <v>0</v>
       </c>
       <c r="Q212" s="1"/>
-    </row>
-    <row r="213" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R212">
+        <v>4181</v>
+      </c>
+      <c r="S212">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="213" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
         <v>106</v>
       </c>
@@ -9296,8 +10443,14 @@
         <v>0</v>
       </c>
       <c r="Q213" s="1"/>
-    </row>
-    <row r="214" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R213">
+        <v>4201</v>
+      </c>
+      <c r="S213">
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="214" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
         <v>202</v>
       </c>
@@ -9332,8 +10485,14 @@
         <v>0</v>
       </c>
       <c r="Q214" s="1"/>
-    </row>
-    <row r="215" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R214">
+        <v>4221</v>
+      </c>
+      <c r="S214">
+        <v>4240</v>
+      </c>
+    </row>
+    <row r="215" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
         <v>203</v>
       </c>
@@ -9368,8 +10527,14 @@
         <v>0</v>
       </c>
       <c r="Q215" s="1"/>
-    </row>
-    <row r="216" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R215">
+        <v>4241</v>
+      </c>
+      <c r="S215">
+        <v>4260</v>
+      </c>
+    </row>
+    <row r="216" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
         <v>132</v>
       </c>
@@ -9404,8 +10569,14 @@
         <v>0</v>
       </c>
       <c r="Q216" s="1"/>
-    </row>
-    <row r="217" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R216">
+        <v>4261</v>
+      </c>
+      <c r="S216">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="217" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>133</v>
       </c>
@@ -9440,8 +10611,14 @@
         <v>0</v>
       </c>
       <c r="Q217" s="1"/>
-    </row>
-    <row r="218" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R217">
+        <v>4281</v>
+      </c>
+      <c r="S217">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="218" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
         <v>134</v>
       </c>
@@ -9476,8 +10653,14 @@
         <v>0</v>
       </c>
       <c r="Q218" s="1"/>
-    </row>
-    <row r="219" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R218">
+        <v>4301</v>
+      </c>
+      <c r="S218">
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="219" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
         <v>204</v>
       </c>
@@ -9512,8 +10695,14 @@
         <v>0</v>
       </c>
       <c r="Q219" s="1"/>
-    </row>
-    <row r="220" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R219">
+        <v>4321</v>
+      </c>
+      <c r="S219">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="220" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
         <v>152</v>
       </c>
@@ -9548,8 +10737,14 @@
         <v>0</v>
       </c>
       <c r="Q220" s="1"/>
-    </row>
-    <row r="221" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R220">
+        <v>4341</v>
+      </c>
+      <c r="S220">
+        <v>4360</v>
+      </c>
+    </row>
+    <row r="221" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
         <v>205</v>
       </c>
@@ -9584,8 +10779,14 @@
         <v>0</v>
       </c>
       <c r="Q221" s="1"/>
-    </row>
-    <row r="222" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R221">
+        <v>4361</v>
+      </c>
+      <c r="S221">
+        <v>4380</v>
+      </c>
+    </row>
+    <row r="222" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
         <v>45</v>
       </c>
@@ -9620,8 +10821,14 @@
         <v>0</v>
       </c>
       <c r="Q222" s="1"/>
-    </row>
-    <row r="223" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R222">
+        <v>4381</v>
+      </c>
+      <c r="S222">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="223" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
         <v>46</v>
       </c>
@@ -9656,8 +10863,14 @@
         <v>0</v>
       </c>
       <c r="Q223" s="1"/>
-    </row>
-    <row r="224" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R223">
+        <v>4401</v>
+      </c>
+      <c r="S223">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="224" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
         <v>245</v>
       </c>
@@ -9692,8 +10905,14 @@
         <v>0</v>
       </c>
       <c r="Q224" s="1"/>
-    </row>
-    <row r="225" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R224">
+        <v>4421</v>
+      </c>
+      <c r="S224">
+        <v>4440</v>
+      </c>
+    </row>
+    <row r="225" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
         <v>78</v>
       </c>
@@ -9728,8 +10947,14 @@
         <v>0</v>
       </c>
       <c r="Q225" s="1"/>
-    </row>
-    <row r="226" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R225">
+        <v>4441</v>
+      </c>
+      <c r="S225">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="226" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
         <v>79</v>
       </c>
@@ -9764,8 +10989,14 @@
         <v>0</v>
       </c>
       <c r="Q226" s="1"/>
-    </row>
-    <row r="227" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R226">
+        <v>4461</v>
+      </c>
+      <c r="S226">
+        <v>4480</v>
+      </c>
+    </row>
+    <row r="227" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
         <v>107</v>
       </c>
@@ -9800,8 +11031,14 @@
         <v>0</v>
       </c>
       <c r="Q227" s="1"/>
-    </row>
-    <row r="228" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R227">
+        <v>4481</v>
+      </c>
+      <c r="S227">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="228" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
         <v>80</v>
       </c>
@@ -9842,8 +11079,14 @@
         <v>0</v>
       </c>
       <c r="Q228" s="1"/>
-    </row>
-    <row r="229" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R228">
+        <v>4501</v>
+      </c>
+      <c r="S228">
+        <v>4520</v>
+      </c>
+    </row>
+    <row r="229" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
         <v>246</v>
       </c>
@@ -9878,8 +11121,14 @@
         <v>0</v>
       </c>
       <c r="Q229" s="1"/>
-    </row>
-    <row r="230" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R229">
+        <v>4521</v>
+      </c>
+      <c r="S229">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="230" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
         <v>108</v>
       </c>
@@ -9914,8 +11163,14 @@
         <v>0</v>
       </c>
       <c r="Q230" s="1"/>
-    </row>
-    <row r="231" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R230">
+        <v>4541</v>
+      </c>
+      <c r="S230">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="231" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
         <v>109</v>
       </c>
@@ -9950,8 +11205,14 @@
         <v>0</v>
       </c>
       <c r="Q231" s="1"/>
-    </row>
-    <row r="232" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R231">
+        <v>4561</v>
+      </c>
+      <c r="S231">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="232" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
         <v>206</v>
       </c>
@@ -9986,8 +11247,14 @@
         <v>0</v>
       </c>
       <c r="Q232" s="1"/>
-    </row>
-    <row r="233" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R232">
+        <v>4581</v>
+      </c>
+      <c r="S232">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="233" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
         <v>207</v>
       </c>
@@ -10022,8 +11289,14 @@
         <v>0</v>
       </c>
       <c r="Q233" s="1"/>
-    </row>
-    <row r="234" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R233">
+        <v>4601</v>
+      </c>
+      <c r="S233">
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="234" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
         <v>135</v>
       </c>
@@ -10058,8 +11331,14 @@
         <v>0</v>
       </c>
       <c r="Q234" s="1"/>
-    </row>
-    <row r="235" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R234">
+        <v>4621</v>
+      </c>
+      <c r="S234">
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="235" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
         <v>81</v>
       </c>
@@ -10094,8 +11373,14 @@
         <v>0</v>
       </c>
       <c r="Q235" s="1"/>
-    </row>
-    <row r="236" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R235">
+        <v>4641</v>
+      </c>
+      <c r="S235">
+        <v>4660</v>
+      </c>
+    </row>
+    <row r="236" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
         <v>247</v>
       </c>
@@ -10130,8 +11415,14 @@
         <v>1</v>
       </c>
       <c r="Q236" s="1"/>
-    </row>
-    <row r="237" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R236">
+        <v>4661</v>
+      </c>
+      <c r="S236">
+        <v>4680</v>
+      </c>
+    </row>
+    <row r="237" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
         <v>248</v>
       </c>
@@ -10166,8 +11457,14 @@
         <v>0</v>
       </c>
       <c r="Q237" s="1"/>
-    </row>
-    <row r="238" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R237">
+        <v>4681</v>
+      </c>
+      <c r="S237">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="238" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
         <v>208</v>
       </c>
@@ -10202,8 +11499,14 @@
         <v>0</v>
       </c>
       <c r="Q238" s="1"/>
-    </row>
-    <row r="239" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R238">
+        <v>4701</v>
+      </c>
+      <c r="S238">
+        <v>4720</v>
+      </c>
+    </row>
+    <row r="239" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
         <v>47</v>
       </c>
@@ -10244,8 +11547,14 @@
         <v>0</v>
       </c>
       <c r="Q239" s="1"/>
-    </row>
-    <row r="240" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R239">
+        <v>4721</v>
+      </c>
+      <c r="S239">
+        <v>4740</v>
+      </c>
+    </row>
+    <row r="240" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
         <v>82</v>
       </c>
@@ -10286,8 +11595,14 @@
         <v>0</v>
       </c>
       <c r="Q240" s="1"/>
-    </row>
-    <row r="241" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R240">
+        <v>4741</v>
+      </c>
+      <c r="S240">
+        <v>4760</v>
+      </c>
+    </row>
+    <row r="241" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
         <v>209</v>
       </c>
@@ -10322,8 +11637,14 @@
         <v>-1</v>
       </c>
       <c r="Q241" s="1"/>
-    </row>
-    <row r="242" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R241">
+        <v>4761</v>
+      </c>
+      <c r="S241">
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="242" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
         <v>48</v>
       </c>
@@ -10358,8 +11679,14 @@
         <v>1</v>
       </c>
       <c r="Q242" s="1"/>
-    </row>
-    <row r="243" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R242">
+        <v>4781</v>
+      </c>
+      <c r="S242">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="243" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
         <v>249</v>
       </c>
@@ -10394,8 +11721,14 @@
         <v>-1</v>
       </c>
       <c r="Q243" s="1"/>
-    </row>
-    <row r="244" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R243">
+        <v>4801</v>
+      </c>
+      <c r="S243">
+        <v>4820</v>
+      </c>
+    </row>
+    <row r="244" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
         <v>153</v>
       </c>
@@ -10430,8 +11763,14 @@
         <v>-1</v>
       </c>
       <c r="Q244" s="1"/>
-    </row>
-    <row r="245" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R244">
+        <v>4821</v>
+      </c>
+      <c r="S244">
+        <v>4840</v>
+      </c>
+    </row>
+    <row r="245" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
         <v>121</v>
       </c>
@@ -10478,8 +11817,14 @@
         <v>1</v>
       </c>
       <c r="Q245" s="1"/>
-    </row>
-    <row r="246" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R245">
+        <v>4841</v>
+      </c>
+      <c r="S245">
+        <v>4860</v>
+      </c>
+    </row>
+    <row r="246" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
         <v>83</v>
       </c>
@@ -10514,8 +11859,14 @@
         <v>0</v>
       </c>
       <c r="Q246" s="1"/>
-    </row>
-    <row r="247" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R246">
+        <v>4861</v>
+      </c>
+      <c r="S246">
+        <v>4880</v>
+      </c>
+    </row>
+    <row r="247" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
         <v>111</v>
       </c>
@@ -10550,8 +11901,14 @@
         <v>0</v>
       </c>
       <c r="Q247" s="1"/>
-    </row>
-    <row r="248" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R247">
+        <v>4881</v>
+      </c>
+      <c r="S247">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="248" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
         <v>154</v>
       </c>
@@ -10586,8 +11943,14 @@
         <v>0</v>
       </c>
       <c r="Q248" s="1"/>
-    </row>
-    <row r="249" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R248">
+        <v>4901</v>
+      </c>
+      <c r="S248">
+        <v>4920</v>
+      </c>
+    </row>
+    <row r="249" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
         <v>210</v>
       </c>
@@ -10622,8 +11985,14 @@
         <v>0</v>
       </c>
       <c r="Q249" s="1"/>
-    </row>
-    <row r="250" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R249">
+        <v>4921</v>
+      </c>
+      <c r="S249">
+        <v>4940</v>
+      </c>
+    </row>
+    <row r="250" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
         <v>110</v>
       </c>
@@ -10658,8 +12027,14 @@
         <v>0</v>
       </c>
       <c r="Q250" s="1"/>
-    </row>
-    <row r="251" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R250">
+        <v>4941</v>
+      </c>
+      <c r="S250">
+        <v>4960</v>
+      </c>
+    </row>
+    <row r="251" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
         <v>84</v>
       </c>
@@ -10694,8 +12069,14 @@
         <v>0</v>
       </c>
       <c r="Q251" s="1"/>
-    </row>
-    <row r="252" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R251">
+        <v>4961</v>
+      </c>
+      <c r="S251">
+        <v>4980</v>
+      </c>
+    </row>
+    <row r="252" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
         <v>211</v>
       </c>
@@ -10730,8 +12111,14 @@
         <v>0</v>
       </c>
       <c r="Q252" s="1"/>
-    </row>
-    <row r="253" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R252">
+        <v>4981</v>
+      </c>
+      <c r="S252">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="253" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
         <v>212</v>
       </c>
@@ -10766,22 +12153,28 @@
         <v>0</v>
       </c>
       <c r="Q253" s="1"/>
+      <c r="R253">
+        <v>5001</v>
+      </c>
+      <c r="S253">
+        <v>5020</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O3:P253">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q253">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
General rework - AZE to BAL
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BB05F7-572B-4C44-B3C8-9F29BCD9950E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6665CF8C-71EC-4FBA-ACC2-C28F0B986F91}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="270">
   <si>
     <t>TAG</t>
   </si>
@@ -893,6 +893,9 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -931,9 +934,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -982,7 +982,7 @@
     <tableColumn id="15" xr3:uid="{AD6381E7-3290-44E4-9E98-E7E9063F54F9}" name="DeltaFM">
       <calculatedColumnFormula>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="0"/>
     <tableColumn id="17" xr3:uid="{C49D052D-3754-49A2-9551-F2176AA27932}" name="ID min"/>
     <tableColumn id="18" xr3:uid="{8A6F4AEA-EC4E-4C6E-A653-1A392AFA8658}" name="ID max"/>
   </tableColumns>
@@ -1256,7 +1256,7 @@
   <dimension ref="A2:R253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,7 +2037,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P18" s="1"/>
+      <c r="P18" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="Q18">
         <v>301</v>
       </c>
@@ -2079,7 +2081,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P19" s="1"/>
+      <c r="P19" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="Q19">
         <v>321</v>
       </c>
@@ -2121,7 +2125,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P20" s="1"/>
+      <c r="P20" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="Q20">
         <v>341</v>
       </c>
@@ -12173,18 +12179,18 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N3:O253">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P253">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Generals rework - separated leaders into own files
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6665CF8C-71EC-4FBA-ACC2-C28F0B986F91}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0ADEEC-B5D2-4E71-BFF3-1B02381B2DAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1256,7 +1256,7 @@
   <dimension ref="A2:R253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,7 +1372,7 @@
         <v>267</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
         <v>20</v>

</xml_diff>